<commit_message>
lots of progress on CDFW landings and life hsitory
</commit_message>
<xml_diff>
--- a/data/landings/mexico/conapesca/raw/CONAPESCA_2015_metadata.xlsx
+++ b/data/landings/mexico/conapesca/raw/CONAPESCA_2015_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/mexico/conapesca/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF00200-7B0A-1447-98E4-713993C967DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C297F32B-68B7-2F43-BFEE-B66E14C98B12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21200" yWindow="620" windowWidth="25600" windowHeight="15540" xr2:uid="{6AD1FC1E-F8F1-934E-8FE7-1FC88D0F3689}"/>
+    <workbookView xWindow="31360" yWindow="7620" windowWidth="25600" windowHeight="15540" xr2:uid="{6AD1FC1E-F8F1-934E-8FE7-1FC88D0F3689}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -836,7 +836,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>